<commit_message>
Changing to work against generic APIs
</commit_message>
<xml_diff>
--- a/APIdef.xlsx
+++ b/APIdef.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28908"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18201"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rjohnson/Projects/APItester/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ron Johnson\projects\APItester\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16240" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="456" windowWidth="28800" windowHeight="16236" tabRatio="500"/>
   </bookViews>
   <sheets>
-    <sheet name="LoadParms" sheetId="2" r:id="rId1"/>
-    <sheet name="config" sheetId="1" r:id="rId2"/>
+    <sheet name="TestAll" sheetId="3" r:id="rId1"/>
+    <sheet name="LoadParms" sheetId="2" r:id="rId2"/>
+    <sheet name="All" sheetId="1" r:id="rId3"/>
   </sheets>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="698" uniqueCount="172">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="714" uniqueCount="176">
   <si>
     <t>ID</t>
   </si>
@@ -544,12 +545,24 @@
   </si>
   <si>
     <t>http://10.20.16.71:8080</t>
+  </si>
+  <si>
+    <t>https://jsonplaceholder.typicode.com</t>
+  </si>
+  <si>
+    <t>/posts</t>
+  </si>
+  <si>
+    <t>userId</t>
+  </si>
+  <si>
+    <t>/posts/{userId}</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -590,6 +603,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -858,29 +874,122 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H21"/>
+  <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G18" sqref="G18"/>
+      <selection pane="bottomLeft" activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="4.1640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.83203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="25.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="2.59765625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.8984375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.5" customWidth="1"/>
+    <col min="6" max="6" width="33" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.59765625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.09765625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="3.19921875" customWidth="1"/>
+    <col min="10" max="10" width="43.796875" customWidth="1"/>
+    <col min="13" max="13" width="138" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>108</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>107</v>
+      </c>
+      <c r="E1" t="s">
+        <v>105</v>
+      </c>
+      <c r="F1" t="s">
+        <v>170</v>
+      </c>
+      <c r="G1" t="s">
+        <v>2</v>
+      </c>
+      <c r="H1" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>110</v>
+      </c>
+      <c r="D2" t="s">
+        <v>174</v>
+      </c>
+      <c r="E2" t="s">
+        <v>174</v>
+      </c>
+      <c r="F2" t="s">
+        <v>172</v>
+      </c>
+      <c r="G2" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>110</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="F3" t="s">
+        <v>172</v>
+      </c>
+      <c r="G3" t="s">
+        <v>175</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H21"/>
+  <sheetViews>
+    <sheetView showRuler="0" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D23" sqref="D23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="4.19921875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.19921875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="25.796875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10.5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20.83203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="62.5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="111.1640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="3.1640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="43.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.796875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="37" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="111.19921875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="3.19921875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="43.796875" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="138" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -906,7 +1015,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>5</v>
       </c>
@@ -929,7 +1038,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>6</v>
       </c>
@@ -952,7 +1061,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>118</v>
       </c>
@@ -972,7 +1081,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>136</v>
       </c>
@@ -995,7 +1104,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>123</v>
       </c>
@@ -1015,7 +1124,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>125</v>
       </c>
@@ -1035,7 +1144,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>128</v>
       </c>
@@ -1055,7 +1164,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>42</v>
       </c>
@@ -1075,7 +1184,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>130</v>
       </c>
@@ -1095,7 +1204,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>44</v>
       </c>
@@ -1115,7 +1224,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>83</v>
       </c>
@@ -1138,7 +1247,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>52</v>
       </c>
@@ -1161,7 +1270,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>65</v>
       </c>
@@ -1184,7 +1293,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>80</v>
       </c>
@@ -1207,7 +1316,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>96</v>
       </c>
@@ -1230,7 +1339,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:7" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>48</v>
       </c>
@@ -1250,7 +1359,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>18</v>
       </c>
@@ -1273,7 +1382,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>8</v>
       </c>
@@ -1296,7 +1405,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>19</v>
       </c>
@@ -1319,7 +1428,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>133</v>
       </c>
@@ -1344,31 +1453,31 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H147"/>
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A120" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G32" sqref="G32"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="4.1640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.83203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="25.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="4.19921875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.19921875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="25.796875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10.5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.796875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="62.5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="111.1640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="3.1640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="43.83203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="111.19921875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="3.19921875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="43.796875" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="138" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1394,7 +1503,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>5</v>
       </c>
@@ -1417,7 +1526,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>6</v>
       </c>
@@ -1440,7 +1549,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>118</v>
       </c>
@@ -1460,7 +1569,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>136</v>
       </c>
@@ -1486,7 +1595,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>123</v>
       </c>
@@ -1506,7 +1615,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>125</v>
       </c>
@@ -1526,7 +1635,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>128</v>
       </c>
@@ -1546,7 +1655,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>42</v>
       </c>
@@ -1566,7 +1675,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>130</v>
       </c>
@@ -1586,7 +1695,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>44</v>
       </c>
@@ -1606,7 +1715,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>83</v>
       </c>
@@ -1629,7 +1738,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>52</v>
       </c>
@@ -1652,7 +1761,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>65</v>
       </c>
@@ -1675,7 +1784,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>80</v>
       </c>
@@ -1698,7 +1807,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>96</v>
       </c>
@@ -1721,7 +1830,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="17" spans="1:8" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:8" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>48</v>
       </c>
@@ -1741,7 +1850,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>18</v>
       </c>
@@ -1764,7 +1873,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>8</v>
       </c>
@@ -1787,7 +1896,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>19</v>
       </c>
@@ -1810,7 +1919,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>133</v>
       </c>
@@ -1830,7 +1939,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>11</v>
       </c>
@@ -1847,7 +1956,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>12</v>
       </c>
@@ -1867,7 +1976,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="24" spans="1:8" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:8" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>22</v>
       </c>
@@ -1887,7 +1996,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>13</v>
       </c>
@@ -1904,7 +2013,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>14</v>
       </c>
@@ -1924,7 +2033,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>15</v>
       </c>
@@ -1941,7 +2050,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>16</v>
       </c>
@@ -1961,7 +2070,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>17</v>
       </c>
@@ -1981,7 +2090,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>20</v>
       </c>
@@ -1998,7 +2107,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>21</v>
       </c>
@@ -2018,7 +2127,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>23</v>
       </c>
@@ -2038,7 +2147,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>24</v>
       </c>
@@ -2058,7 +2167,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>9</v>
       </c>
@@ -2075,7 +2184,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>10</v>
       </c>
@@ -2095,7 +2204,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>25</v>
       </c>
@@ -2112,7 +2221,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>32</v>
       </c>
@@ -2129,7 +2238,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>43</v>
       </c>
@@ -2146,7 +2255,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>47</v>
       </c>
@@ -2163,7 +2272,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>51</v>
       </c>
@@ -2180,7 +2289,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>55</v>
       </c>
@@ -2200,7 +2309,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>56</v>
       </c>
@@ -2217,7 +2326,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>57</v>
       </c>
@@ -2234,7 +2343,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>58</v>
       </c>
@@ -2254,7 +2363,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>59</v>
       </c>
@@ -2274,7 +2383,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>60</v>
       </c>
@@ -2294,7 +2403,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>61</v>
       </c>
@@ -2311,7 +2420,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>62</v>
       </c>
@@ -2328,7 +2437,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>63</v>
       </c>
@@ -2345,7 +2454,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>64</v>
       </c>
@@ -2362,7 +2471,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A51">
         <v>66</v>
       </c>
@@ -2379,7 +2488,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A52">
         <v>67</v>
       </c>
@@ -2396,7 +2505,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A53">
         <v>68</v>
       </c>
@@ -2413,7 +2522,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A54">
         <v>69</v>
       </c>
@@ -2430,7 +2539,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A55">
         <v>70</v>
       </c>
@@ -2447,7 +2556,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A56">
         <v>71</v>
       </c>
@@ -2467,7 +2576,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A57">
         <v>72</v>
       </c>
@@ -2487,7 +2596,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A58">
         <v>73</v>
       </c>
@@ -2504,7 +2613,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A59">
         <v>75</v>
       </c>
@@ -2521,7 +2630,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A60">
         <v>76</v>
       </c>
@@ -2538,7 +2647,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A61">
         <v>77</v>
       </c>
@@ -2555,7 +2664,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A62">
         <v>84</v>
       </c>
@@ -2572,7 +2681,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A63">
         <v>85</v>
       </c>
@@ -2592,7 +2701,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A64">
         <v>86</v>
       </c>
@@ -2609,7 +2718,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A65">
         <v>87</v>
       </c>
@@ -2629,7 +2738,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A66">
         <v>88</v>
       </c>
@@ -2646,7 +2755,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A67">
         <v>89</v>
       </c>
@@ -2666,7 +2775,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A68">
         <v>90</v>
       </c>
@@ -2683,7 +2792,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A69">
         <v>91</v>
       </c>
@@ -2703,7 +2812,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A70">
         <v>92</v>
       </c>
@@ -2723,7 +2832,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A71">
         <v>93</v>
       </c>
@@ -2740,7 +2849,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A72">
         <v>94</v>
       </c>
@@ -2757,7 +2866,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A73">
         <v>95</v>
       </c>
@@ -2774,7 +2883,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A74">
         <v>53</v>
       </c>
@@ -2794,7 +2903,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A75">
         <v>97</v>
       </c>
@@ -2811,7 +2920,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A76">
         <v>119</v>
       </c>
@@ -2828,7 +2937,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A77">
         <v>124</v>
       </c>
@@ -2845,7 +2954,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A78">
         <v>126</v>
       </c>
@@ -2862,7 +2971,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A79">
         <v>129</v>
       </c>
@@ -2879,7 +2988,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A80">
         <v>131</v>
       </c>
@@ -2896,7 +3005,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A81">
         <v>135</v>
       </c>
@@ -2913,7 +3022,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A82">
         <v>137</v>
       </c>
@@ -2930,7 +3039,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A83">
         <v>138</v>
       </c>
@@ -2947,7 +3056,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A84">
         <v>139</v>
       </c>
@@ -2967,7 +3076,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A85">
         <v>98</v>
       </c>
@@ -2987,7 +3096,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="86" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A86">
         <v>106</v>
       </c>
@@ -3004,7 +3113,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A87">
         <v>107</v>
       </c>
@@ -3021,7 +3130,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="88" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A88">
         <v>108</v>
       </c>
@@ -3041,7 +3150,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="89" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A89">
         <v>109</v>
       </c>
@@ -3061,7 +3170,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="90" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A90">
         <v>110</v>
       </c>
@@ -3081,7 +3190,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="91" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A91">
         <v>111</v>
       </c>
@@ -3101,7 +3210,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="92" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A92">
         <v>132</v>
       </c>
@@ -3118,7 +3227,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="93" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A93">
         <v>33</v>
       </c>
@@ -3138,7 +3247,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="94" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A94">
         <v>34</v>
       </c>
@@ -3158,7 +3267,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="95" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A95">
         <v>12</v>
       </c>
@@ -3178,7 +3287,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="96" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A96">
         <v>13</v>
       </c>
@@ -3198,7 +3307,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="97" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A97">
         <v>14</v>
       </c>
@@ -3218,7 +3327,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="98" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A98">
         <v>54</v>
       </c>
@@ -3238,7 +3347,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="99" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A99">
         <v>74</v>
       </c>
@@ -3258,7 +3367,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="100" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A100">
         <v>1</v>
       </c>
@@ -3275,7 +3384,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="101" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A101">
         <v>2</v>
       </c>
@@ -3292,7 +3401,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="102" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A102">
         <v>3</v>
       </c>
@@ -3309,7 +3418,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="103" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A103">
         <v>4</v>
       </c>
@@ -3326,7 +3435,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="104" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A104">
         <v>7</v>
       </c>
@@ -3343,7 +3452,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="105" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A105">
         <v>31</v>
       </c>
@@ -3357,7 +3466,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="106" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A106">
         <v>35</v>
       </c>
@@ -3371,7 +3480,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="107" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A107">
         <v>36</v>
       </c>
@@ -3388,7 +3497,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="108" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A108">
         <v>37</v>
       </c>
@@ -3405,7 +3514,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="109" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A109">
         <v>38</v>
       </c>
@@ -3422,7 +3531,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="110" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A110">
         <v>39</v>
       </c>
@@ -3439,7 +3548,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="111" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A111">
         <v>40</v>
       </c>
@@ -3456,7 +3565,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="112" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A112">
         <v>41</v>
       </c>
@@ -3470,7 +3579,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="113" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A113">
         <v>45</v>
       </c>
@@ -3487,7 +3596,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="114" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A114">
         <v>46</v>
       </c>
@@ -3504,7 +3613,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="115" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A115">
         <v>49</v>
       </c>
@@ -3521,7 +3630,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="116" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A116">
         <v>50</v>
       </c>
@@ -3538,7 +3647,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="117" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A117">
         <v>78</v>
       </c>
@@ -3552,7 +3661,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="118" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A118">
         <v>79</v>
       </c>
@@ -3569,7 +3678,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="119" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A119">
         <v>81</v>
       </c>
@@ -3586,7 +3695,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="120" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A120">
         <v>82</v>
       </c>
@@ -3603,7 +3712,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="121" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A121">
         <v>99</v>
       </c>
@@ -3620,7 +3729,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="122" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A122">
         <v>100</v>
       </c>
@@ -3637,7 +3746,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="123" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A123">
         <v>101</v>
       </c>
@@ -3654,7 +3763,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="124" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A124">
         <v>102</v>
       </c>
@@ -3671,7 +3780,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="125" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A125">
         <v>103</v>
       </c>
@@ -3688,7 +3797,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="126" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A126">
         <v>104</v>
       </c>
@@ -3705,7 +3814,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="127" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A127">
         <v>105</v>
       </c>
@@ -3722,7 +3831,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="128" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A128">
         <v>112</v>
       </c>
@@ -3736,7 +3845,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="129" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A129">
         <v>113</v>
       </c>
@@ -3750,7 +3859,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="130" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A130">
         <v>114</v>
       </c>
@@ -3767,7 +3876,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="131" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A131">
         <v>115</v>
       </c>
@@ -3784,7 +3893,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="132" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A132">
         <v>116</v>
       </c>
@@ -3801,7 +3910,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="133" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A133">
         <v>117</v>
       </c>
@@ -3815,7 +3924,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="134" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A134">
         <v>120</v>
       </c>
@@ -3829,7 +3938,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="135" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A135">
         <v>121</v>
       </c>
@@ -3843,7 +3952,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="136" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A136">
         <v>122</v>
       </c>
@@ -3860,7 +3969,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="137" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A137">
         <v>127</v>
       </c>
@@ -3877,7 +3986,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="138" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A138">
         <v>134</v>
       </c>
@@ -3894,7 +4003,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="139" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A139">
         <v>140</v>
       </c>
@@ -3908,7 +4017,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="140" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A140">
         <v>141</v>
       </c>
@@ -3925,7 +4034,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="141" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A141">
         <v>142</v>
       </c>
@@ -3942,7 +4051,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="142" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A142">
         <v>143</v>
       </c>
@@ -3959,7 +4068,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="143" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A143">
         <v>144</v>
       </c>
@@ -3976,7 +4085,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="144" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A144">
         <v>145</v>
       </c>
@@ -3993,7 +4102,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="145" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A145">
         <v>146</v>
       </c>
@@ -4010,7 +4119,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="146" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A146">
         <v>147</v>
       </c>
@@ -4027,7 +4136,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="147" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A147">
         <v>148</v>
       </c>

</xml_diff>